<commit_message>
STAM table put back to its original state
</commit_message>
<xml_diff>
--- a/src/Data/STAM_table.xlsx
+++ b/src/Data/STAM_table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA35F4D9-8D6F-4436-A9E5-0AAAD18796D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52E771E-EB6C-4843-A07B-65D34494CBDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>Agriculture</t>
   </si>
@@ -593,7 +593,7 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +739,7 @@
       <c r="R2" s="2">
         <v>1</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="7">
         <v>1</v>
       </c>
       <c r="T2" s="2">
@@ -810,7 +810,7 @@
       <c r="R3" s="2">
         <v>1</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="7">
         <v>1</v>
       </c>
       <c r="T3" s="2">
@@ -881,7 +881,7 @@
       <c r="R4" s="2">
         <v>1</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="7">
         <v>1</v>
       </c>
       <c r="T4" s="2">
@@ -952,7 +952,7 @@
       <c r="R5" s="2">
         <v>1</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="7">
         <v>1</v>
       </c>
       <c r="T5" s="2">
@@ -1023,7 +1023,7 @@
       <c r="R6" s="12">
         <v>1</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="7">
         <v>1</v>
       </c>
       <c r="T6" s="2">
@@ -1094,7 +1094,7 @@
       <c r="R7" s="2">
         <v>1</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="7">
         <v>1</v>
       </c>
       <c r="T7" s="2">
@@ -1165,7 +1165,7 @@
       <c r="R8" s="12">
         <v>1</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="7">
         <v>1</v>
       </c>
       <c r="T8" s="2">
@@ -1236,7 +1236,7 @@
       <c r="R9" s="2">
         <v>1</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="7">
         <v>1</v>
       </c>
       <c r="T9" s="2">
@@ -1307,7 +1307,7 @@
       <c r="R10" s="2">
         <v>1</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="7">
         <v>1</v>
       </c>
       <c r="T10" s="2">
@@ -2276,5 +2276,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Disaggregated computers and furnitures from machineries
</commit_message>
<xml_diff>
--- a/src/Data/STAM_table.xlsx
+++ b/src/Data/STAM_table.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52E771E-EB6C-4843-A07B-65D34494CBDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9D69E8-BE55-4295-9A7B-DBDD0CDED3D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22260" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Agriculture</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Metal products</t>
-  </si>
-  <si>
-    <t>Machinery</t>
   </si>
   <si>
     <t>Construction</t>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>Electricity/heat</t>
+  </si>
+  <si>
+    <t>Office equipment</t>
+  </si>
+  <si>
+    <t>Machinery</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -183,19 +186,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -205,21 +195,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -237,12 +212,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF00B050"/>
       </left>
-      <right style="medium">
-        <color rgb="FF00B050"/>
-      </right>
+      <right/>
       <top style="medium">
         <color rgb="FF00B050"/>
       </top>
@@ -251,11 +235,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -288,28 +305,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,13 +634,14 @@
     <col min="15" max="15" width="10.33203125" customWidth="1"/>
     <col min="16" max="16" width="21.77734375" customWidth="1"/>
     <col min="17" max="17" width="13.77734375" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="16.109375" customWidth="1"/>
+    <col min="18" max="18" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.21875" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
@@ -630,34 +655,34 @@
         <v>3</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="I1" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="L1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>5</v>
@@ -665,26 +690,29 @@
       <c r="Q1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -736,13 +764,13 @@
       <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="7">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
+      <c r="R2" s="7">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="7">
         <v>1</v>
       </c>
       <c r="U2" s="2">
@@ -754,8 +782,11 @@
       <c r="W2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -804,16 +835,16 @@
       <c r="P3" s="2">
         <v>1</v>
       </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-      <c r="R3" s="2">
-        <v>1</v>
-      </c>
-      <c r="S3" s="7">
-        <v>1</v>
-      </c>
-      <c r="T3" s="2">
+      <c r="Q3" s="13">
+        <v>1</v>
+      </c>
+      <c r="R3" s="7">
+        <v>1</v>
+      </c>
+      <c r="S3" s="11">
+        <v>1</v>
+      </c>
+      <c r="T3" s="7">
         <v>1</v>
       </c>
       <c r="U3" s="2">
@@ -825,8 +856,11 @@
       <c r="W3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -875,16 +909,16 @@
       <c r="P4" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="2">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2">
-        <v>1</v>
-      </c>
-      <c r="S4" s="7">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2">
+      <c r="Q4" s="13">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7">
+        <v>1</v>
+      </c>
+      <c r="S4" s="11">
+        <v>1</v>
+      </c>
+      <c r="T4" s="7">
         <v>1</v>
       </c>
       <c r="U4" s="2">
@@ -896,8 +930,11 @@
       <c r="W4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -946,174 +983,183 @@
       <c r="P5" s="2">
         <v>1</v>
       </c>
-      <c r="Q5" s="14">
-        <v>1</v>
-      </c>
-      <c r="R5" s="2">
-        <v>1</v>
-      </c>
-      <c r="S5" s="7">
-        <v>1</v>
-      </c>
-      <c r="T5" s="2">
+      <c r="Q5" s="17">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7">
+        <v>1</v>
+      </c>
+      <c r="S5" s="11">
+        <v>1</v>
+      </c>
+      <c r="T5" s="7">
         <v>1</v>
       </c>
       <c r="U5" s="2">
         <v>1</v>
       </c>
-      <c r="V5" s="4">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>0</v>
+      </c>
+      <c r="R6" s="7">
+        <v>1</v>
+      </c>
+      <c r="S6" s="11">
+        <v>1</v>
+      </c>
+      <c r="T6" s="7">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
-      <c r="P6" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>0</v>
-      </c>
-      <c r="R6" s="12">
-        <v>1</v>
-      </c>
-      <c r="S6" s="7">
-        <v>1</v>
-      </c>
-      <c r="T6" s="2">
-        <v>1</v>
-      </c>
-      <c r="U6" s="2">
-        <v>1</v>
-      </c>
-      <c r="V6" s="2">
-        <v>1</v>
-      </c>
-      <c r="W6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="19">
+        <v>1</v>
+      </c>
+      <c r="R7" s="7">
+        <v>1</v>
+      </c>
+      <c r="S7" s="11">
+        <v>1</v>
+      </c>
+      <c r="T7" s="7">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="17">
-        <v>1</v>
-      </c>
-      <c r="R7" s="2">
-        <v>1</v>
-      </c>
-      <c r="S7" s="7">
-        <v>1</v>
-      </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
@@ -1156,19 +1202,19 @@
       <c r="O8" s="3">
         <v>0</v>
       </c>
-      <c r="P8" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="15">
-        <v>0</v>
-      </c>
-      <c r="R8" s="12">
-        <v>1</v>
-      </c>
-      <c r="S8" s="7">
-        <v>1</v>
-      </c>
-      <c r="T8" s="2">
+      <c r="P8" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>0</v>
+      </c>
+      <c r="R8" s="7">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7">
         <v>1</v>
       </c>
       <c r="U8" s="2">
@@ -1180,10 +1226,13 @@
       <c r="W8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1230,16 +1279,16 @@
       <c r="P9" s="2">
         <v>1</v>
       </c>
-      <c r="Q9" s="11">
-        <v>1</v>
-      </c>
-      <c r="R9" s="2">
-        <v>1</v>
-      </c>
-      <c r="S9" s="7">
-        <v>1</v>
-      </c>
-      <c r="T9" s="2">
+      <c r="Q9" s="21">
+        <v>1</v>
+      </c>
+      <c r="R9" s="7">
+        <v>1</v>
+      </c>
+      <c r="S9" s="11">
+        <v>1</v>
+      </c>
+      <c r="T9" s="7">
         <v>1</v>
       </c>
       <c r="U9" s="2">
@@ -1251,82 +1300,88 @@
       <c r="W9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7">
+        <v>1</v>
+      </c>
+      <c r="S10" s="11">
+        <v>1</v>
+      </c>
+      <c r="T10" s="7">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2">
+        <v>1</v>
+      </c>
+      <c r="X10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="N10" s="2">
-        <v>1</v>
-      </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2">
-        <v>1</v>
-      </c>
-      <c r="S10" s="7">
-        <v>1</v>
-      </c>
-      <c r="T10" s="2">
-        <v>1</v>
-      </c>
-      <c r="U10" s="2">
-        <v>1</v>
-      </c>
-      <c r="V10" s="2">
-        <v>1</v>
-      </c>
-      <c r="W10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
@@ -1372,20 +1427,20 @@
       <c r="P11" s="2">
         <v>1</v>
       </c>
-      <c r="Q11" s="2">
-        <v>1</v>
-      </c>
-      <c r="R11" s="2">
-        <v>1</v>
-      </c>
-      <c r="S11" s="2">
-        <v>1</v>
-      </c>
-      <c r="T11" s="3">
-        <v>0</v>
-      </c>
-      <c r="U11" s="2">
-        <v>1</v>
+      <c r="Q11" s="13">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="11">
+        <v>1</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
       </c>
       <c r="V11" s="2">
         <v>1</v>
@@ -1393,10 +1448,13 @@
       <c r="W11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -1443,13 +1501,13 @@
       <c r="P12" s="2">
         <v>1</v>
       </c>
-      <c r="Q12" s="2">
-        <v>1</v>
-      </c>
-      <c r="R12" s="2">
-        <v>1</v>
-      </c>
-      <c r="S12" s="2">
+      <c r="Q12" s="13">
+        <v>1</v>
+      </c>
+      <c r="R12" s="7">
+        <v>1</v>
+      </c>
+      <c r="S12" s="11">
         <v>1</v>
       </c>
       <c r="T12" s="2">
@@ -1464,8 +1522,11 @@
       <c r="W12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1514,20 +1575,20 @@
       <c r="P13" s="2">
         <v>1</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="13">
         <v>1</v>
       </c>
       <c r="R13" s="3">
         <v>0</v>
       </c>
-      <c r="S13" s="2">
-        <v>1</v>
-      </c>
-      <c r="T13" s="3">
-        <v>0</v>
-      </c>
-      <c r="U13" s="2">
-        <v>1</v>
+      <c r="S13" s="22">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>1</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0</v>
       </c>
       <c r="V13" s="2">
         <v>1</v>
@@ -1535,10 +1596,13 @@
       <c r="W13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
@@ -1588,7 +1652,7 @@
       <c r="Q14" s="2">
         <v>1</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="7">
         <v>1</v>
       </c>
       <c r="S14" s="2">
@@ -1606,10 +1670,13 @@
       <c r="W14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1659,7 +1726,7 @@
       <c r="Q15" s="3">
         <v>0</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="7">
         <v>1</v>
       </c>
       <c r="S15" s="2">
@@ -1677,8 +1744,11 @@
       <c r="W15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1730,17 +1800,17 @@
       <c r="Q16" s="2">
         <v>1</v>
       </c>
-      <c r="R16" s="3">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>1</v>
+      <c r="R16" s="7">
+        <v>1</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
       </c>
       <c r="V16" s="2">
         <v>1</v>
@@ -1748,8 +1818,11 @@
       <c r="W16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1804,14 +1877,14 @@
       <c r="R17" s="3">
         <v>0</v>
       </c>
-      <c r="S17" s="2">
-        <v>1</v>
-      </c>
-      <c r="T17" s="3">
-        <v>0</v>
-      </c>
-      <c r="U17" s="2">
-        <v>1</v>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0</v>
       </c>
       <c r="V17" s="2">
         <v>1</v>
@@ -1819,460 +1892,559 @@
       <c r="W17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="X17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <v>1</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1</v>
+      </c>
+      <c r="X18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1</v>
+      </c>
+      <c r="R19" s="7">
+        <v>1</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2">
+        <v>1</v>
+      </c>
+      <c r="W19" s="2">
+        <v>1</v>
+      </c>
+      <c r="X19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>1</v>
+      </c>
+      <c r="R20" s="7">
+        <v>1</v>
+      </c>
+      <c r="S20" s="2">
+        <v>1</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1</v>
+      </c>
+      <c r="V20" s="2">
+        <v>1</v>
+      </c>
+      <c r="W20" s="4">
+        <v>0</v>
+      </c>
+      <c r="X20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1</v>
-      </c>
-      <c r="M18" s="2">
-        <v>1</v>
-      </c>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="O18" s="2">
-        <v>1</v>
-      </c>
-      <c r="P18" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>1</v>
-      </c>
-      <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="4">
-        <v>0</v>
-      </c>
-      <c r="T18" s="2">
-        <v>1</v>
-      </c>
-      <c r="U18" s="2">
-        <v>1</v>
-      </c>
-      <c r="V18" s="2">
-        <v>1</v>
-      </c>
-      <c r="W18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1</v>
-      </c>
-      <c r="J19" s="2">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2">
-        <v>1</v>
-      </c>
-      <c r="L19" s="2">
-        <v>1</v>
-      </c>
-      <c r="M19" s="2">
-        <v>1</v>
-      </c>
-      <c r="N19" s="2">
-        <v>1</v>
-      </c>
-      <c r="O19" s="2">
-        <v>1</v>
-      </c>
-      <c r="P19" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
-      <c r="R19" s="2">
-        <v>1</v>
-      </c>
-      <c r="S19" s="2">
-        <v>1</v>
-      </c>
-      <c r="T19" s="2">
-        <v>1</v>
-      </c>
-      <c r="U19" s="2">
-        <v>1</v>
-      </c>
-      <c r="V19" s="4">
-        <v>0</v>
-      </c>
-      <c r="W19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
+        <v>1</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="7">
+        <v>1</v>
+      </c>
+      <c r="S21" s="2">
+        <v>1</v>
+      </c>
+      <c r="T21" s="2">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
+        <v>1</v>
+      </c>
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1</v>
-      </c>
-      <c r="K20" s="2">
-        <v>1</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" s="2">
-        <v>1</v>
-      </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
-      <c r="O20" s="2">
-        <v>1</v>
-      </c>
-      <c r="P20" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>1</v>
-      </c>
-      <c r="R20" s="2">
-        <v>1</v>
-      </c>
-      <c r="S20" s="2">
-        <v>1</v>
-      </c>
-      <c r="T20" s="2">
-        <v>1</v>
-      </c>
-      <c r="U20" s="2">
-        <v>1</v>
-      </c>
-      <c r="V20" s="2">
-        <v>1</v>
-      </c>
-      <c r="W20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="7">
+        <v>1</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1</v>
+      </c>
+      <c r="U22" s="2">
+        <v>1</v>
+      </c>
+      <c r="V22" s="2">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2">
+        <v>1</v>
+      </c>
+      <c r="X22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
+        <v>1</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1</v>
+      </c>
+      <c r="U23" s="2">
+        <v>1</v>
+      </c>
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
+      <c r="W23" s="2">
+        <v>1</v>
+      </c>
+      <c r="X23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2">
-        <v>1</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1</v>
-      </c>
-      <c r="M21" s="2">
-        <v>1</v>
-      </c>
-      <c r="N21" s="2">
-        <v>1</v>
-      </c>
-      <c r="O21" s="2">
-        <v>1</v>
-      </c>
-      <c r="P21" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>1</v>
-      </c>
-      <c r="R21" s="2">
-        <v>1</v>
-      </c>
-      <c r="S21" s="2">
-        <v>1</v>
-      </c>
-      <c r="T21" s="2">
-        <v>1</v>
-      </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
-      <c r="V21" s="2">
-        <v>1</v>
-      </c>
-      <c r="W21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1</v>
-      </c>
-      <c r="J22" s="2">
-        <v>1</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
-      </c>
-      <c r="M22" s="2">
-        <v>1</v>
-      </c>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
-      <c r="O22" s="2">
-        <v>1</v>
-      </c>
-      <c r="P22" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>1</v>
-      </c>
-      <c r="R22" s="2">
-        <v>1</v>
-      </c>
-      <c r="S22" s="2">
-        <v>1</v>
-      </c>
-      <c r="T22" s="2">
-        <v>1</v>
-      </c>
-      <c r="U22" s="2">
-        <v>1</v>
-      </c>
-      <c r="V22" s="2">
-        <v>1</v>
-      </c>
-      <c r="W22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
-        <v>1</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1</v>
-      </c>
-      <c r="M23" s="2">
-        <v>1</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23" s="2">
-        <v>1</v>
-      </c>
-      <c r="P23" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>1</v>
-      </c>
-      <c r="R23" s="2">
-        <v>1</v>
-      </c>
-      <c r="S23" s="2">
-        <v>1</v>
-      </c>
-      <c r="T23" s="2">
-        <v>1</v>
-      </c>
-      <c r="U23" s="2">
-        <v>1</v>
-      </c>
-      <c r="V23" s="2">
-        <v>1</v>
-      </c>
-      <c r="W23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1</v>
+      </c>
+      <c r="R24" s="7">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1</v>
+      </c>
+      <c r="T24" s="2">
+        <v>1</v>
+      </c>
+      <c r="U24" s="2">
+        <v>1</v>
+      </c>
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
+      <c r="W24" s="2">
+        <v>1</v>
+      </c>
+      <c r="X24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D26" s="6"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D27" s="6"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="14"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="D28" s="6"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="14"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="14"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>